<commit_message>
Corrected small errors in QWET exercise
</commit_message>
<xml_diff>
--- a/Materials/Shahe_data/shahe_data.xlsx
+++ b/Materials/Shahe_data/shahe_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/tkan_dtu_dk/Documents/WET_teaching material/Nanjing_workshop-2024/Exercises/shahe_data_upd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkan\repos\wet-workshop\Materials\Shahe_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="11_2737DA81459C5F8E5DC8096E4FE9678023773D92" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AC852D8-4586-4735-8E34-D88198DA7AC9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AE342A-21C6-4D9F-95EA-FFD96DB03EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" tabRatio="693" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="693" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Physical_domain" sheetId="23" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Longitude</t>
   </si>
@@ -85,16 +85,7 @@
     <t>turbulence &gt; turb_param</t>
   </si>
   <si>
-    <t>cSigTm</t>
-  </si>
-  <si>
-    <t>cTmOpt</t>
-  </si>
-  <si>
     <t>/day</t>
-  </si>
-  <si>
-    <t>degree Celsius</t>
   </si>
   <si>
     <t>m2/s2</t>
@@ -962,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -1106,7 +1097,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1125,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1144,7 +1135,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1157,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1976D054-AE7C-4BE9-B07A-9865BCDD4821}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1184,48 +1175,26 @@
         <v>13</v>
       </c>
       <c r="C4" s="4">
-        <v>4.1899999999999997E-6</v>
+        <v>4.8999999999999997E-6</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>